<commit_message>
Time Record Manager - 5th July 2024
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTI0045472_VerifyBetaUserWithDifferentTitleIsAbletoEnterHoursfromTimeRecordmanager.xlsx
+++ b/TestData/LV_TMTI0045472_VerifyBetaUserWithDifferentTitleIsAbletoEnterHoursfromTimeRecordmanager.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9197034E-90B3-4784-BECF-244FC8C85B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8594CA8-AAA6-42CF-8C2E-16BD9360E9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -458,15 +458,15 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -480,7 +480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -494,7 +494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -522,14 +522,14 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -543,18 +543,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C4EBE5-CDA0-489C-820D-6ED5D2289F5E}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -572,14 +575,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -601,7 +604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -625,16 +628,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +652,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -666,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -693,19 +696,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -730,7 +733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -744,7 +747,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
     </row>
   </sheetData>

</xml_diff>